<commit_message>
Adding Rol/Usuario/LogEvento Services and ApiControllers
</commit_message>
<xml_diff>
--- a/PVenta BD/PVenta.xlsx
+++ b/PVenta BD/PVenta.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DesaVisual\PVenta\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DesaVisual\PVenta\PVenta BD\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14595" windowHeight="4545" firstSheet="11" activeTab="15"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14595" windowHeight="4545" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="EstructuraSist" sheetId="1" r:id="rId1"/>
@@ -346,11 +346,11 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1455,33 +1455,33 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="C4" s="6">
+      <c r="B4" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" s="5">
         <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="C5" s="6"/>
+      <c r="C5" s="5"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="C6" s="5">
+      <c r="C6" s="4">
         <v>16.2</v>
       </c>
     </row>
@@ -1621,7 +1621,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
@@ -1631,11 +1631,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="6" t="s">
         <v>61</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
+      <c r="B2" s="6"/>
+      <c r="C2" s="6"/>
       <c r="D2" s="2">
         <f>SUM(D3:D9)</f>
         <v>12552</v>
@@ -1907,8 +1907,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1933,10 +1933,10 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="5" t="s">
+      <c r="A3" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="4" t="s">
         <v>49</v>
       </c>
       <c r="C3" s="1"/>
@@ -1954,7 +1954,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B5" t="s">
         <v>50</v>

</xml_diff>

<commit_message>
Change Model OpcionesSist, fixed service OpcionesSist and Api Controller OpcionesSist
</commit_message>
<xml_diff>
--- a/PVenta BD/PVenta.xlsx
+++ b/PVenta BD/PVenta.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14595" windowHeight="4545" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14595" windowHeight="4545" firstSheet="3" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="EstructuraSist" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="324" uniqueCount="79">
   <si>
     <t>Roles</t>
   </si>
@@ -273,6 +273,9 @@
   </si>
   <si>
     <t>RolId</t>
+  </si>
+  <si>
+    <t>Codigo</t>
   </si>
 </sst>
 </file>
@@ -341,7 +344,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -349,6 +352,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1907,7 +1913,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
@@ -2020,18 +2026,26 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <sheetPr>
+    <tabColor rgb="FFC00000"/>
+  </sheetPr>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="7" t="s">
         <v>10</v>
       </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -2054,24 +2068,38 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>78</v>
       </c>
       <c r="B4" t="s">
         <v>50</v>
       </c>
       <c r="C4">
-        <v>50</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
         <v>56</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2081,7 +2109,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Changin BD File Excel - OpcionesSist
</commit_message>
<xml_diff>
--- a/PVenta BD/PVenta.xlsx
+++ b/PVenta BD/PVenta.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14595" windowHeight="4545" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14595" windowHeight="4545"/>
   </bookViews>
   <sheets>
     <sheet name="EstructuraSist" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="79">
   <si>
     <t>Roles</t>
   </si>
@@ -273,13 +273,16 @@
   </si>
   <si>
     <t>RolId</t>
+  </si>
+  <si>
+    <t>Codigo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -320,6 +323,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="16"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -338,10 +358,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -351,8 +372,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -633,66 +659,66 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.28515625" customWidth="1"/>
-    <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="8" max="9" width="17" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17.85546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:14" ht="21" x14ac:dyDescent="0.35">
+      <c r="A1" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="L1" s="3" t="s">
+      <c r="L1" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="M1" s="3" t="s">
+      <c r="M1" s="8" t="s">
         <v>31</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="N1" s="8" t="s">
         <v>33</v>
       </c>
     </row>
@@ -751,7 +777,7 @@
         <v>6</v>
       </c>
       <c r="D3" t="s">
-        <v>11</v>
+        <v>78</v>
       </c>
       <c r="E3" t="s">
         <v>15</v>
@@ -795,7 +821,7 @@
         <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="E4" t="s">
         <v>4</v>
@@ -838,6 +864,9 @@
       <c r="C5" t="s">
         <v>12</v>
       </c>
+      <c r="D5" t="s">
+        <v>4</v>
+      </c>
       <c r="G5" t="s">
         <v>4</v>
       </c>
@@ -949,6 +978,22 @@
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" location="'1. LogEventos'!A1" display="LogEventos"/>
+    <hyperlink ref="B1" location="'2. Roles'!A1" display="Roles"/>
+    <hyperlink ref="C1" location="'3. Usuarios'!A1" display="Usuarios"/>
+    <hyperlink ref="D1" location="'4. OpcionesSist'!A1" display="OpcionesSist"/>
+    <hyperlink ref="E1" location="'5. PermisosRoles'!A1" display="PermisosRoles"/>
+    <hyperlink ref="F1" location="'6. Mesas'!A1" display="Mesas"/>
+    <hyperlink ref="G1" location="'7. Monedas'!A1" display="Monedas"/>
+    <hyperlink ref="H1" location="'8. Categorias'!A1" display="Categorias"/>
+    <hyperlink ref="I1" location="'9. Productos'!A1" display="Productos"/>
+    <hyperlink ref="J1" location="'10. FacturaHeader'!A1" display="FacturaHeader"/>
+    <hyperlink ref="K1" location="'11. FacturaDetail'!A1" display="FacturaDetail"/>
+    <hyperlink ref="L1" location="'12. FacturaPayment'!A1" display="FacturaPayment"/>
+    <hyperlink ref="M1" location="'13. CuadreHeader'!A1" display="CuadreHeader"/>
+    <hyperlink ref="N1" location="'14. CuadreDetail'!A1" display="CuadreDetail"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1758,9 +1803,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1907,7 +1950,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
@@ -2020,18 +2063,26 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <sheetPr>
+    <tabColor rgb="FFC00000"/>
+  </sheetPr>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="7" t="s">
         <v>10</v>
       </c>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
@@ -2054,24 +2105,38 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>78</v>
       </c>
       <c r="B4" t="s">
         <v>50</v>
       </c>
       <c r="C4">
-        <v>50</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C5">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
         <v>56</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2081,7 +2146,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update file PVenta.xlsx BD
</commit_message>
<xml_diff>
--- a/PVenta BD/PVenta.xlsx
+++ b/PVenta BD/PVenta.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14595" windowHeight="4545"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14595" windowHeight="4545" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="EstructuraSist" sheetId="1" r:id="rId1"/>
@@ -369,13 +369,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -659,7 +659,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -679,46 +679,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="D1" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="E1" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="G1" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H1" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="I1" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="J1" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="K1" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="L1" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="M1" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="N1" s="8" t="s">
+      <c r="N1" s="6" t="s">
         <v>33</v>
       </c>
     </row>
@@ -1001,6 +1001,9 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFFFF00"/>
+  </sheetPr>
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1108,6 +1111,9 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFF0000"/>
+  </sheetPr>
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1253,6 +1259,9 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFF0000"/>
+  </sheetPr>
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1368,6 +1377,9 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFF0000"/>
+  </sheetPr>
   <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1464,9 +1476,12 @@
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFF0000"/>
+  </sheetPr>
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -1584,10 +1599,13 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFF0000"/>
+  </sheetPr>
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1676,11 +1694,11 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
       <c r="D2" s="2">
         <f>SUM(D3:D9)</f>
         <v>12552</v>
@@ -1801,6 +1819,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FF92D050"/>
+  </sheetPr>
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -1879,6 +1900,9 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FF92D050"/>
+  </sheetPr>
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1948,10 +1972,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FF92D050"/>
+  </sheetPr>
   <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2064,12 +2091,12 @@
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
-    <tabColor rgb="FFC00000"/>
+    <tabColor rgb="FF92D050"/>
   </sheetPr>
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2143,6 +2170,9 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFFFF00"/>
+  </sheetPr>
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2198,6 +2228,9 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFFFF00"/>
+  </sheetPr>
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2259,6 +2292,9 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFFFF00"/>
+  </sheetPr>
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2331,6 +2367,9 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFFFF00"/>
+  </sheetPr>
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>